<commit_message>
renamed implementation date to effective date
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
+++ b/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DA077-8BC7-4F90-AFDA-7B79C63F0291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,7 +34,7 @@
     <t>announcement_date</t>
   </si>
   <si>
-    <t>implementation_date</t>
+    <t>effective_date</t>
   </si>
   <si>
     <t>ADDED</t>
@@ -1105,11 +1111,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1173,6 +1179,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1219,7 +1233,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1251,9 +1265,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,6 +1317,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1460,14 +1510,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="17.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.41796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1504,7 +1558,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1524,7 +1578,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1544,7 +1598,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1564,7 +1618,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1584,7 +1638,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1604,7 +1658,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1624,7 +1678,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1644,7 +1698,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1664,7 +1718,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1684,7 +1738,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1704,7 +1758,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1724,7 +1778,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1744,7 +1798,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1764,7 +1818,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1784,7 +1838,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1804,7 +1858,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1824,7 +1878,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1844,7 +1898,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1864,7 +1918,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1884,7 +1938,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1904,7 +1958,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1924,7 +1978,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1944,7 +1998,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1964,7 +2018,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1984,7 +2038,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2004,7 +2058,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2024,7 +2078,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2044,7 +2098,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2064,7 +2118,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2084,7 +2138,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2104,7 +2158,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2124,7 +2178,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2144,7 +2198,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2164,7 +2218,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2184,7 +2238,7 @@
         <v>42307</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2204,7 +2258,7 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2224,7 +2278,7 @@
         <v>42317</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2244,7 +2298,7 @@
         <v>42318</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2264,7 +2318,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2284,7 +2338,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2304,7 +2358,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2324,7 +2378,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2344,7 +2398,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2364,7 +2418,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2384,7 +2438,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2404,7 +2458,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2424,7 +2478,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2444,7 +2498,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2464,7 +2518,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2484,7 +2538,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2504,7 +2558,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2524,7 +2578,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2544,7 +2598,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2564,7 +2618,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2584,7 +2638,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2604,7 +2658,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2624,7 +2678,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2644,7 +2698,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2664,7 +2718,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2684,7 +2738,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2704,7 +2758,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2724,7 +2778,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2744,7 +2798,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2764,7 +2818,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2784,7 +2838,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2804,7 +2858,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2824,7 +2878,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2844,7 +2898,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2864,7 +2918,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2884,7 +2938,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2904,7 +2958,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2924,7 +2978,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2944,7 +2998,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2964,7 +3018,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2984,7 +3038,7 @@
         <v>42552</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3004,7 +3058,7 @@
         <v>42556</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3024,7 +3078,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3044,7 +3098,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3064,7 +3118,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3084,7 +3138,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3104,7 +3158,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3124,7 +3178,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3144,7 +3198,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3164,7 +3218,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3184,7 +3238,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3204,7 +3258,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3224,7 +3278,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3244,7 +3298,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3264,7 +3318,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3284,7 +3338,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3304,7 +3358,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3324,7 +3378,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3344,7 +3398,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3364,7 +3418,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3384,7 +3438,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3404,7 +3458,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3424,7 +3478,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3444,7 +3498,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3464,7 +3518,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3484,7 +3538,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3504,7 +3558,7 @@
         <v>42954</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3524,7 +3578,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3544,7 +3598,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3564,7 +3618,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3584,7 +3638,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3604,7 +3658,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3624,7 +3678,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3644,7 +3698,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3664,7 +3718,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3684,7 +3738,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3704,7 +3758,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3724,7 +3778,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3744,7 +3798,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3764,7 +3818,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3784,7 +3838,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3804,7 +3858,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3824,7 +3878,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3844,7 +3898,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3864,7 +3918,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3884,7 +3938,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3904,7 +3958,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3924,7 +3978,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3944,7 +3998,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3964,7 +4018,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3984,7 +4038,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4004,7 +4058,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4024,7 +4078,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4044,7 +4098,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4064,7 +4118,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4084,7 +4138,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4104,7 +4158,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4124,7 +4178,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4144,7 +4198,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4164,7 +4218,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4184,7 +4238,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4204,7 +4258,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4224,7 +4278,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4244,7 +4298,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4264,7 +4318,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4284,7 +4338,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4304,7 +4358,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4324,7 +4378,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4344,7 +4398,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4364,7 +4418,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4384,7 +4438,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4404,7 +4458,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4424,7 +4478,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4444,7 +4498,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4464,7 +4518,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4484,7 +4538,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -4504,7 +4558,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -4524,7 +4578,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -4544,7 +4598,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4564,7 +4618,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -4584,7 +4638,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -4604,7 +4658,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4624,7 +4678,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4644,7 +4698,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4664,7 +4718,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4684,7 +4738,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4704,7 +4758,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4724,7 +4778,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4744,7 +4798,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4764,7 +4818,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4784,7 +4838,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4804,7 +4858,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4824,7 +4878,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4844,7 +4898,7 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4864,7 +4918,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4884,7 +4938,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4904,7 +4958,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4924,7 +4978,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4944,7 +4998,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4964,7 +5018,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -4984,7 +5038,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -5004,7 +5058,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -5024,7 +5078,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -5044,7 +5098,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5064,7 +5118,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -5084,7 +5138,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -5104,7 +5158,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -5124,7 +5178,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -5144,7 +5198,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -5164,7 +5218,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -5184,7 +5238,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -5204,7 +5258,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -5224,7 +5278,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -5244,7 +5298,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -5264,7 +5318,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
improved accuracy by limiting to 20 characters before bracket
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
+++ b/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yingchen\Documents\GitHub\analyzingalpha\sp500-historical-components-and-changes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C4A0E9-570C-4A58-A6C0-E00BF446A6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18276" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -721,7 +715,7 @@
     <t>CB</t>
   </si>
   <si>
-    <t>CRAY</t>
+    <t>FRT</t>
   </si>
   <si>
     <t>BRCM</t>
@@ -1123,11 +1117,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1191,14 +1185,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1245,7 +1231,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1277,27 +1263,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1329,24 +1297,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1522,16 +1472,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1568,7 +1516,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1588,7 +1536,7 @@
         <v>43734</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1608,7 +1556,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1628,7 +1576,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1648,7 +1596,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1668,7 +1616,7 @@
         <v>43804</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1688,7 +1636,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1708,7 +1656,7 @@
         <v>43808</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1728,7 +1676,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1748,7 +1696,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1768,7 +1716,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1788,7 +1736,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1808,7 +1756,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1828,7 +1776,7 @@
         <v>43822</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1848,7 +1796,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1868,7 +1816,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1888,7 +1836,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1908,7 +1856,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1928,7 +1876,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1948,7 +1896,7 @@
         <v>43924</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1968,7 +1916,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1988,7 +1936,7 @@
         <v>43927</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2008,7 +1956,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2028,7 +1976,7 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2048,7 +1996,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2068,7 +2016,7 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2088,7 +2036,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2108,7 +2056,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2128,7 +2076,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2148,7 +2096,7 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2168,7 +2116,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2188,7 +2136,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2208,7 +2156,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2228,7 +2176,7 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2248,7 +2196,7 @@
         <v>42307</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2268,7 +2216,7 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2288,7 +2236,7 @@
         <v>42317</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2308,7 +2256,7 @@
         <v>42318</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2328,7 +2276,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2348,7 +2296,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2368,7 +2316,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2388,7 +2336,7 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2408,7 +2356,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2428,7 +2376,7 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2448,7 +2396,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2468,7 +2416,7 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2488,7 +2436,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2508,7 +2456,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2528,7 +2476,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2548,7 +2496,7 @@
         <v>42398</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2568,7 +2516,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:6">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2588,7 +2536,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2608,7 +2556,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:6">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2628,7 +2576,7 @@
         <v>42432</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:6">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2648,7 +2596,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2668,7 +2616,7 @@
         <v>42433</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:6">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2688,7 +2636,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:6">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2708,7 +2656,7 @@
         <v>42461</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:6">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2728,7 +2676,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:6">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2748,7 +2696,7 @@
         <v>42475</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2768,7 +2716,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:6">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2788,7 +2736,7 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:6">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2828,7 +2776,7 @@
         <v>42502</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2848,7 +2796,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2868,7 +2816,7 @@
         <v>42507</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2888,7 +2836,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2908,7 +2856,7 @@
         <v>42510</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2928,7 +2876,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2948,7 +2896,7 @@
         <v>42517</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2968,7 +2916,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2988,7 +2936,7 @@
         <v>42544</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:6">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3008,7 +2956,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:6">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3028,7 +2976,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:6">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3048,7 +2996,7 @@
         <v>42552</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:6">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3068,7 +3016,7 @@
         <v>42556</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:6">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3088,7 +3036,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:6">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3108,7 +3056,7 @@
         <v>42551</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:6">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3128,7 +3076,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:6">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3148,7 +3096,7 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:6">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3168,7 +3116,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:6">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3188,7 +3136,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:6">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3208,7 +3156,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:6">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3228,7 +3176,7 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:6">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3248,7 +3196,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:6">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3268,7 +3216,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:6">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3288,7 +3236,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:6">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3308,7 +3256,7 @@
         <v>42829</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:6">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3328,7 +3276,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:6">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3348,7 +3296,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:6">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3368,7 +3316,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:6">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3388,7 +3336,7 @@
         <v>42888</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:6">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3408,7 +3356,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:6">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3428,7 +3376,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:6">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3448,7 +3396,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:6">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3468,7 +3416,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:6">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3488,7 +3436,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:6">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3508,7 +3456,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:6">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3528,7 +3476,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:6">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3548,7 +3496,7 @@
         <v>42905</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:6">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3568,7 +3516,7 @@
         <v>42954</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:6">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3588,7 +3536,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:6">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3608,7 +3556,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:6">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3628,7 +3576,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:6">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3648,7 +3596,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:6">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3668,7 +3616,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:6">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3688,7 +3636,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:6">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3708,7 +3656,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:6">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3728,7 +3676,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:6">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3748,7 +3696,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:6">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3768,7 +3716,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:6">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3788,7 +3736,7 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:6">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3808,7 +3756,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:6">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3828,7 +3776,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:6">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3848,7 +3796,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:6">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3868,7 +3816,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:6">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3888,7 +3836,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:6">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3908,7 +3856,7 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:6">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3928,7 +3876,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:6">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3948,7 +3896,7 @@
         <v>43166</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:6">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3968,7 +3916,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:6">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3988,7 +3936,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:6">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4008,7 +3956,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:6">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4028,7 +3976,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:6">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4048,7 +3996,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:6">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4068,7 +4016,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:6">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4088,7 +4036,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:6">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4108,7 +4056,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:6">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4128,7 +4076,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:6">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4148,7 +4096,7 @@
         <v>43258</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:6">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4168,7 +4116,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:6">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4188,7 +4136,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:6">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4208,7 +4156,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:6">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4228,7 +4176,7 @@
         <v>43269</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:6">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4248,7 +4196,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:6">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4268,7 +4216,7 @@
         <v>43271</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:6">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4288,7 +4236,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:6">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4308,7 +4256,7 @@
         <v>43283</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:6">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4328,7 +4276,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:6">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4348,7 +4296,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:6">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4368,7 +4316,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:6">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4388,7 +4336,7 @@
         <v>43360</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:6">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4408,7 +4356,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:6">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4428,7 +4376,7 @@
         <v>43374</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:6">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4448,7 +4396,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:6">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4468,7 +4416,7 @@
         <v>43384</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:6">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4488,7 +4436,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:6">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4508,7 +4456,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:6">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4528,7 +4476,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:6">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4548,7 +4496,7 @@
         <v>43417</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:6">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -4568,7 +4516,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:6">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -4588,7 +4536,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:6">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -4608,7 +4556,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:6">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4628,7 +4576,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:6">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -4648,7 +4596,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:6">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -4668,7 +4616,7 @@
         <v>43437</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:6">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4688,7 +4636,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:6">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4708,7 +4656,7 @@
         <v>43458</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:6">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4728,7 +4676,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:6">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4748,7 +4696,7 @@
         <v>43467</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:6">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4768,7 +4716,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:6">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4788,7 +4736,7 @@
         <v>43483</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:6">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4808,7 +4756,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:6">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4828,7 +4776,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:6">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4848,7 +4796,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:6">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4868,7 +4816,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:6">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4888,7 +4836,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:6">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4908,7 +4856,7 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:6">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4928,7 +4876,7 @@
         <v>43557</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:6">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4948,7 +4896,7 @@
         <v>43558</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:6">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4968,7 +4916,7 @@
         <v>43619</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:6">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4988,7 +4936,7 @@
         <v>43620</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:6">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -5008,7 +4956,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:6">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -5028,7 +4976,7 @@
         <v>43623</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:6">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -5048,7 +4996,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:6">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -5068,7 +5016,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:6">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -5088,7 +5036,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:6">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -5108,7 +5056,7 @@
         <v>43661</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:6">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5128,7 +5076,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:6">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -5148,7 +5096,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:6">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -5168,7 +5116,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:6">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -5188,7 +5136,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:6">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -5208,7 +5156,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:6">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -5228,7 +5176,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:6">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -5248,7 +5196,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:6">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -5268,7 +5216,7 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:6">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -5288,7 +5236,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:6">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -5308,7 +5256,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:6">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -5328,7 +5276,7 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:6">
       <c r="A191" s="1">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
split into implementation and effective dates
</commit_message>
<xml_diff>
--- a/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
+++ b/sp500-historical-components-and-changes/sp500_rebalance_announcements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="367">
   <si>
     <t>type</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>announcement_date</t>
+  </si>
+  <si>
+    <t>implementation_date</t>
   </si>
   <si>
     <t>effective_date</t>
@@ -1473,13 +1476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:G191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1495,459 +1498,462 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
         <v>43728</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>43734</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E3" s="2">
         <v>43728</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>43734</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E4" s="2">
         <v>43734</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>43741</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E5" s="2">
         <v>43734</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E6" s="2">
         <v>43796</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>43804</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E7" s="2">
         <v>43796</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>43804</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E8" s="2">
         <v>43801</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>43808</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E9" s="2">
         <v>43801</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>43808</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E10" s="2">
         <v>43812</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E11" s="2">
         <v>43812</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E12" s="2">
         <v>43812</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E13" s="2">
         <v>43812</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E14" s="2">
         <v>43812</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E15" s="2">
         <v>43812</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>43822</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E16" s="2">
         <v>43852</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>43858</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E17" s="2">
         <v>43852</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>43858</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E18" s="2">
         <v>43888</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>43893</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E19" s="2">
         <v>43888</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>43893</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E20" s="2">
         <v>43921</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>43924</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E21" s="2">
         <v>43921</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>43924</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E22" s="2">
         <v>43921</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>43927</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E23" s="2">
         <v>43921</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>43927</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E24" s="2">
         <v>41397</v>
@@ -1956,18 +1962,18 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E25" s="2">
         <v>41397</v>
@@ -1976,18 +1982,18 @@
         <v>41402</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E26" s="2">
         <v>41410</v>
@@ -1996,18 +2002,18 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E27" s="2">
         <v>41410</v>
@@ -2016,18 +2022,18 @@
         <v>41417</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E28" s="2">
         <v>42072</v>
@@ -2036,18 +2042,18 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E29" s="2">
         <v>42072</v>
@@ -2056,18 +2062,18 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E30" s="2">
         <v>42164</v>
@@ -2076,18 +2082,18 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E31" s="2">
         <v>42164</v>
@@ -2096,58 +2102,58 @@
         <v>42166</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E32" s="2">
         <v>43097</v>
       </c>
-      <c r="F32" s="2">
+      <c r="G32" s="2">
         <v>43103</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E33" s="2">
         <v>43097</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>43103</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E34" s="2">
         <v>42277</v>
@@ -2156,18 +2162,18 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E35" s="2">
         <v>42277</v>
@@ -2176,18 +2182,18 @@
         <v>42284</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E36" s="2">
         <v>42304</v>
@@ -2196,18 +2202,18 @@
         <v>42307</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E37" s="2">
         <v>42304</v>
@@ -2216,18 +2222,18 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E38" s="2">
         <v>42310</v>
@@ -2236,18 +2242,18 @@
         <v>42317</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E39" s="2">
         <v>42310</v>
@@ -2256,18 +2262,18 @@
         <v>42318</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E40" s="2">
         <v>42317</v>
@@ -2276,18 +2282,18 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E41" s="2">
         <v>42317</v>
@@ -2296,18 +2302,18 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E42" s="2">
         <v>42320</v>
@@ -2316,18 +2322,18 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D43" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E43" s="2">
         <v>42320</v>
@@ -2336,18 +2342,18 @@
         <v>42326</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E44" s="2">
         <v>42366</v>
@@ -2356,18 +2362,18 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E45" s="2">
         <v>42366</v>
@@ -2376,18 +2382,18 @@
         <v>42373</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E46" s="2">
         <v>42382</v>
@@ -2396,18 +2402,18 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E47" s="2">
         <v>42382</v>
@@ -2416,18 +2422,18 @@
         <v>42384</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E48" s="2">
         <v>42391</v>
@@ -2441,13 +2447,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E49" s="2">
         <v>42391</v>
@@ -2461,13 +2467,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E50" s="2">
         <v>42395</v>
@@ -2481,13 +2487,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E51" s="2">
         <v>42395</v>
@@ -2501,13 +2507,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D52" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E52" s="2">
         <v>42416</v>
@@ -2521,13 +2527,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D53" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E53" s="2">
         <v>42416</v>
@@ -2541,13 +2547,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D54" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E54" s="2">
         <v>42430</v>
@@ -2561,13 +2567,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D55" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E55" s="2">
         <v>42430</v>
@@ -2581,13 +2587,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D56" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E56" s="2">
         <v>42432</v>
@@ -2601,13 +2607,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D57" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E57" s="2">
         <v>42432</v>
@@ -2621,13 +2627,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E58" s="2">
         <v>42457</v>
@@ -2641,13 +2647,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E59" s="2">
         <v>42457</v>
@@ -2661,13 +2667,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E60" s="2">
         <v>42467</v>
@@ -2681,13 +2687,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E61" s="2">
         <v>42467</v>
@@ -2701,13 +2707,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D62" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E62" s="2">
         <v>42479</v>
@@ -2721,13 +2727,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D63" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E63" s="2">
         <v>42479</v>
@@ -2741,13 +2747,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E64" s="2">
         <v>42500</v>
@@ -2761,13 +2767,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E65" s="2">
         <v>42500</v>
@@ -2781,13 +2787,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E66" s="2">
         <v>42503</v>
@@ -2801,13 +2807,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E67" s="2">
         <v>42503</v>
@@ -2821,13 +2827,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E68" s="2">
         <v>42508</v>
@@ -2841,13 +2847,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D69" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E69" s="2">
         <v>42508</v>
@@ -2861,13 +2867,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D70" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E70" s="2">
         <v>42514</v>
@@ -2881,13 +2887,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E71" s="2">
         <v>42514</v>
@@ -2901,13 +2907,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D72" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E72" s="2">
         <v>42542</v>
@@ -2921,13 +2927,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D73" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E73" s="2">
         <v>42542</v>
@@ -2941,13 +2947,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E74" s="2">
         <v>42544</v>
@@ -2961,13 +2967,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E75" s="2">
         <v>42544</v>
@@ -2981,13 +2987,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D76" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E76" s="2">
         <v>42544</v>
@@ -3001,13 +3007,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D77" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E77" s="2">
         <v>42544</v>
@@ -3021,13 +3027,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D78" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E78" s="2">
         <v>42550</v>
@@ -3041,13 +3047,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D79" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E79" s="2">
         <v>42550</v>
@@ -3061,13 +3067,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D80" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E80" s="2">
         <v>42607</v>
@@ -3076,18 +3082,18 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D81" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E81" s="2">
         <v>42607</v>
@@ -3096,18 +3102,18 @@
         <v>42615</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C82" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D82" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E82" s="2">
         <v>42640</v>
@@ -3116,18 +3122,18 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D83" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E83" s="2">
         <v>42640</v>
@@ -3136,18 +3142,18 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D84" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E84" s="2">
         <v>42738</v>
@@ -3156,18 +3162,18 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E85" s="2">
         <v>42738</v>
@@ -3176,538 +3182,538 @@
         <v>42739</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D86" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E86" s="2">
         <v>42800</v>
       </c>
-      <c r="F86" s="2">
+      <c r="G86" s="2">
         <v>42807</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D87" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E87" s="2">
         <v>42800</v>
       </c>
-      <c r="F87" s="2">
+      <c r="G87" s="2">
         <v>42807</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D88" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E88" s="2">
         <v>42822</v>
       </c>
-      <c r="F88" s="2">
+      <c r="G88" s="2">
         <v>42829</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D89" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E89" s="2">
         <v>42822</v>
       </c>
-      <c r="F89" s="2">
+      <c r="G89" s="2">
         <v>42829</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:7">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E90" s="2">
         <v>42823</v>
       </c>
-      <c r="F90" s="2">
+      <c r="G90" s="2">
         <v>42830</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:7">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D91" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E91" s="2">
         <v>42823</v>
       </c>
-      <c r="F91" s="2">
+      <c r="G91" s="2">
         <v>42830</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D92" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E92" s="2">
         <v>42879</v>
       </c>
-      <c r="F92" s="2">
+      <c r="G92" s="2">
         <v>42888</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D93" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E93" s="2">
         <v>42879</v>
       </c>
-      <c r="F93" s="2">
+      <c r="G93" s="2">
         <v>42888</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D94" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E94" s="2">
         <v>42895</v>
       </c>
-      <c r="F94" s="2">
+      <c r="G94" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D95" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E95" s="2">
         <v>42895</v>
       </c>
-      <c r="F95" s="2">
+      <c r="G95" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D96" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E96" s="2">
         <v>42895</v>
       </c>
-      <c r="F96" s="2">
+      <c r="G96" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C97" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D97" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E97" s="2">
         <v>42895</v>
       </c>
-      <c r="F97" s="2">
+      <c r="G97" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E98" s="2">
         <v>42895</v>
       </c>
-      <c r="F98" s="2">
+      <c r="G98" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:7">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D99" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E99" s="2">
         <v>42895</v>
       </c>
-      <c r="F99" s="2">
+      <c r="G99" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:7">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C100" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E100" s="2">
         <v>42898</v>
       </c>
-      <c r="F100" s="2">
+      <c r="G100" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:7">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C101" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D101" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E101" s="2">
         <v>42898</v>
       </c>
-      <c r="F101" s="2">
+      <c r="G101" s="2">
         <v>42905</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:7">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D102" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E102" s="2">
         <v>42947</v>
       </c>
-      <c r="F102" s="2">
+      <c r="G102" s="2">
         <v>42954</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:7">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C103" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D103" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E103" s="2">
         <v>42947</v>
       </c>
-      <c r="F103" s="2">
+      <c r="G103" s="2">
         <v>42955</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:7">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D104" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E104" s="2">
         <v>42971</v>
       </c>
-      <c r="F104" s="2">
+      <c r="G104" s="2">
         <v>42976</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:7">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C105" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D105" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E105" s="2">
         <v>42971</v>
       </c>
-      <c r="F105" s="2">
+      <c r="G105" s="2">
         <v>42976</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:7">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D106" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E106" s="2">
         <v>42971</v>
       </c>
-      <c r="F106" s="2">
+      <c r="G106" s="2">
         <v>42979</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:7">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D107" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E107" s="2">
         <v>42971</v>
       </c>
-      <c r="F107" s="2">
+      <c r="G107" s="2">
         <v>42979</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:7">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D108" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="E108" s="2">
         <v>42986</v>
       </c>
-      <c r="F108" s="2">
+      <c r="G108" s="2">
         <v>42996</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:7">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D109" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E109" s="2">
         <v>42986</v>
       </c>
-      <c r="F109" s="2">
+      <c r="G109" s="2">
         <v>42996</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:7">
       <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C110" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D110" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E110" s="2">
         <v>43012</v>
       </c>
-      <c r="F110" s="2">
+      <c r="G110" s="2">
         <v>43021</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:7">
       <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C111" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D111" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E111" s="2">
         <v>43012</v>
       </c>
-      <c r="F111" s="2">
+      <c r="G111" s="2">
         <v>43021</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:7">
       <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C112" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D112" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="E112" s="2">
         <v>41600</v>
@@ -3716,18 +3722,18 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:7">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D113" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E113" s="2">
         <v>41600</v>
@@ -3736,18 +3742,18 @@
         <v>41607</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:7">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D114" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E114" s="2">
         <v>41619</v>
@@ -3756,18 +3762,18 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:7">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D115" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E115" s="2">
         <v>41619</v>
@@ -3776,18 +3782,18 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:7">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D116" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E116" s="2">
         <v>41619</v>
@@ -3796,18 +3802,18 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:7">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C117" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D117" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E117" s="2">
         <v>41619</v>
@@ -3816,18 +3822,18 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:7">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C118" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D118" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E118" s="2">
         <v>41619</v>
@@ -3836,18 +3842,18 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:7">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D119" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E119" s="2">
         <v>41619</v>
@@ -3856,1298 +3862,1298 @@
         <v>41628</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:7">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C120" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D120" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E120" s="2">
         <v>43161</v>
       </c>
-      <c r="F120" s="2">
+      <c r="G120" s="2">
         <v>43166</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:7">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D121" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E121" s="2">
         <v>43161</v>
       </c>
-      <c r="F121" s="2">
+      <c r="G121" s="2">
         <v>43166</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:7">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C122" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D122" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E122" s="2">
         <v>43168</v>
       </c>
-      <c r="F122" s="2">
+      <c r="G122" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:7">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D123" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E123" s="2">
         <v>43168</v>
       </c>
-      <c r="F123" s="2">
+      <c r="G123" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:7">
       <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E124" s="2">
         <v>43168</v>
       </c>
-      <c r="F124" s="2">
+      <c r="G124" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:7">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C125" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D125" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E125" s="2">
         <v>43168</v>
       </c>
-      <c r="F125" s="2">
+      <c r="G125" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:7">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D126" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E126" s="2">
         <v>43168</v>
       </c>
-      <c r="F126" s="2">
+      <c r="G126" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:7">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C127" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D127" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E127" s="2">
         <v>43168</v>
       </c>
-      <c r="F127" s="2">
+      <c r="G127" s="2">
         <v>43178</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:7">
       <c r="A128" s="1">
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D128" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E128" s="2">
         <v>43245</v>
       </c>
-      <c r="F128" s="2">
+      <c r="G128" s="2">
         <v>43251</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:7">
       <c r="A129" s="1">
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C129" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D129" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E129" s="2">
         <v>43245</v>
       </c>
-      <c r="F129" s="2">
+      <c r="G129" s="2">
         <v>43251</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:7">
       <c r="A130" s="1">
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C130" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D130" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E130" s="2">
         <v>43255</v>
       </c>
-      <c r="F130" s="2">
+      <c r="G130" s="2">
         <v>43258</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:7">
       <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C131" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D131" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E131" s="2">
         <v>43255</v>
       </c>
-      <c r="F131" s="2">
+      <c r="G131" s="2">
         <v>43258</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:7">
       <c r="A132" s="1">
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C132" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D132" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="E132" s="2">
         <v>43259</v>
       </c>
-      <c r="F132" s="2">
+      <c r="G132" s="2">
         <v>43269</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:7">
       <c r="A133" s="1">
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C133" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D133" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E133" s="2">
         <v>43259</v>
       </c>
-      <c r="F133" s="2">
+      <c r="G133" s="2">
         <v>43269</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:7">
       <c r="A134" s="1">
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C134" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D134" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E134" s="2">
         <v>43259</v>
       </c>
-      <c r="F134" s="2">
+      <c r="G134" s="2">
         <v>43269</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:7">
       <c r="A135" s="1">
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D135" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E135" s="2">
         <v>43259</v>
       </c>
-      <c r="F135" s="2">
+      <c r="G135" s="2">
         <v>43269</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:7">
       <c r="A136" s="1">
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C136" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D136" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E136" s="2">
         <v>43266</v>
       </c>
-      <c r="F136" s="2">
+      <c r="G136" s="2">
         <v>43271</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:7">
       <c r="A137" s="1">
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C137" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D137" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="E137" s="2">
         <v>43266</v>
       </c>
-      <c r="F137" s="2">
+      <c r="G137" s="2">
         <v>43271</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:7">
       <c r="A138" s="1">
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C138" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D138" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E138" s="2">
         <v>43276</v>
       </c>
-      <c r="F138" s="2">
+      <c r="G138" s="2">
         <v>43283</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:7">
       <c r="A139" s="1">
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C139" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D139" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E139" s="2">
         <v>43276</v>
       </c>
-      <c r="F139" s="2">
+      <c r="G139" s="2">
         <v>43283</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:7">
       <c r="A140" s="1">
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D140" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E140" s="2">
         <v>43335</v>
       </c>
-      <c r="F140" s="2">
+      <c r="G140" s="2">
         <v>43340</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:7">
       <c r="A141" s="1">
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C141" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D141" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E141" s="2">
         <v>43335</v>
       </c>
-      <c r="F141" s="2">
+      <c r="G141" s="2">
         <v>43340</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:7">
       <c r="A142" s="1">
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E142" s="2">
         <v>43354</v>
       </c>
-      <c r="F142" s="2">
+      <c r="G142" s="2">
         <v>43360</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:7">
       <c r="A143" s="1">
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C143" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D143" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="E143" s="2">
         <v>43354</v>
       </c>
-      <c r="F143" s="2">
+      <c r="G143" s="2">
         <v>43360</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:7">
       <c r="A144" s="1">
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D144" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E144" s="2">
         <v>43368</v>
       </c>
-      <c r="F144" s="2">
+      <c r="G144" s="2">
         <v>43374</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:7">
       <c r="A145" s="1">
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C145" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D145" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E145" s="2">
         <v>43368</v>
       </c>
-      <c r="F145" s="2">
+      <c r="G145" s="2">
         <v>43374</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:7">
       <c r="A146" s="1">
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D146" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E146" s="2">
         <v>43377</v>
       </c>
-      <c r="F146" s="2">
+      <c r="G146" s="2">
         <v>43384</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:7">
       <c r="A147" s="1">
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C147" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D147" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E147" s="2">
         <v>43377</v>
       </c>
-      <c r="F147" s="2">
+      <c r="G147" s="2">
         <v>43384</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:7">
       <c r="A148" s="1">
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D148" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E148" s="2">
         <v>43403</v>
       </c>
-      <c r="F148" s="2">
+      <c r="G148" s="2">
         <v>43410</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:7">
       <c r="A149" s="1">
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C149" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D149" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E149" s="2">
         <v>43403</v>
       </c>
-      <c r="F149" s="2">
+      <c r="G149" s="2">
         <v>43410</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:7">
       <c r="A150" s="1">
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D150" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E150" s="2">
         <v>43411</v>
       </c>
-      <c r="F150" s="2">
+      <c r="G150" s="2">
         <v>43417</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:7">
       <c r="A151" s="1">
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C151" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D151" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E151" s="2">
         <v>43411</v>
       </c>
-      <c r="F151" s="2">
+      <c r="G151" s="2">
         <v>43417</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:7">
       <c r="A152" s="1">
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D152" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E152" s="2">
         <v>43430</v>
       </c>
-      <c r="F152" s="2">
+      <c r="G152" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:7">
       <c r="A153" s="1">
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D153" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="E153" s="2">
         <v>43430</v>
       </c>
-      <c r="F153" s="2">
+      <c r="G153" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:7">
       <c r="A154" s="1">
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D154" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E154" s="2">
         <v>43430</v>
       </c>
-      <c r="F154" s="2">
+      <c r="G154" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:7">
       <c r="A155" s="1">
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C155" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D155" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E155" s="2">
         <v>43430</v>
       </c>
-      <c r="F155" s="2">
+      <c r="G155" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:7">
       <c r="A156" s="1">
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C156" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D156" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E156" s="2">
         <v>43430</v>
       </c>
-      <c r="F156" s="2">
+      <c r="G156" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:7">
       <c r="A157" s="1">
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C157" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D157" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E157" s="2">
         <v>43430</v>
       </c>
-      <c r="F157" s="2">
+      <c r="G157" s="2">
         <v>43437</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:7">
       <c r="A158" s="1">
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C158" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D158" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E158" s="2">
         <v>43453</v>
       </c>
-      <c r="F158" s="2">
+      <c r="G158" s="2">
         <v>43458</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:7">
       <c r="A159" s="1">
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D159" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E159" s="2">
         <v>43453</v>
       </c>
-      <c r="F159" s="2">
+      <c r="G159" s="2">
         <v>43458</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:7">
       <c r="A160" s="1">
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C160" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D160" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E160" s="2">
         <v>43461</v>
       </c>
-      <c r="F160" s="2">
+      <c r="G160" s="2">
         <v>43467</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:7">
       <c r="A161" s="1">
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D161" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E161" s="2">
         <v>43461</v>
       </c>
-      <c r="F161" s="2">
+      <c r="G161" s="2">
         <v>43467</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:7">
       <c r="A162" s="1">
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C162" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D162" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E162" s="2">
         <v>43480</v>
       </c>
-      <c r="F162" s="2">
+      <c r="G162" s="2">
         <v>43483</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:7">
       <c r="A163" s="1">
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C163" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D163" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E163" s="2">
         <v>43480</v>
       </c>
-      <c r="F163" s="2">
+      <c r="G163" s="2">
         <v>43483</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:7">
       <c r="A164" s="1">
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C164" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D164" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E164" s="2">
         <v>43504</v>
       </c>
-      <c r="F164" s="2">
+      <c r="G164" s="2">
         <v>43511</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:7">
       <c r="A165" s="1">
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C165" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D165" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E165" s="2">
         <v>43504</v>
       </c>
-      <c r="F165" s="2">
+      <c r="G165" s="2">
         <v>43511</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:7">
       <c r="A166" s="1">
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C166" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D166" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E166" s="2">
         <v>43517</v>
       </c>
-      <c r="F166" s="2">
+      <c r="G166" s="2">
         <v>43523</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:7">
       <c r="A167" s="1">
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D167" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="E167" s="2">
         <v>43517</v>
       </c>
-      <c r="F167" s="2">
+      <c r="G167" s="2">
         <v>43523</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:7">
       <c r="A168" s="1">
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C168" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D168" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E168" s="2">
         <v>43538</v>
       </c>
-      <c r="F168" s="2">
+      <c r="G168" s="2">
         <v>43543</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:7">
       <c r="A169" s="1">
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C169" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D169" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E169" s="2">
         <v>43538</v>
       </c>
-      <c r="F169" s="2">
+      <c r="G169" s="2">
         <v>43544</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:7">
       <c r="A170" s="1">
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C170" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D170" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E170" s="2">
         <v>43550</v>
       </c>
-      <c r="F170" s="2">
+      <c r="G170" s="2">
         <v>43557</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:7">
       <c r="A171" s="1">
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C171" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D171" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E171" s="2">
         <v>43550</v>
       </c>
-      <c r="F171" s="2">
+      <c r="G171" s="2">
         <v>43558</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:7">
       <c r="A172" s="1">
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C172" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D172" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="E172" s="2">
         <v>43613</v>
       </c>
-      <c r="F172" s="2">
+      <c r="G172" s="2">
         <v>43619</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:7">
       <c r="A173" s="1">
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C173" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D173" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E173" s="2">
         <v>43613</v>
       </c>
-      <c r="F173" s="2">
+      <c r="G173" s="2">
         <v>43620</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:7">
       <c r="A174" s="1">
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C174" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D174" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E174" s="2">
         <v>43619</v>
       </c>
-      <c r="F174" s="2">
+      <c r="G174" s="2">
         <v>43623</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:7">
       <c r="A175" s="1">
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C175" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D175" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E175" s="2">
         <v>43619</v>
       </c>
-      <c r="F175" s="2">
+      <c r="G175" s="2">
         <v>43623</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:7">
       <c r="A176" s="1">
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C176" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D176" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E176" s="2">
         <v>43640</v>
       </c>
-      <c r="F176" s="2">
+      <c r="G176" s="2">
         <v>43647</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:7">
       <c r="A177" s="1">
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C177" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D177" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E177" s="2">
         <v>43640</v>
       </c>
-      <c r="F177" s="2">
+      <c r="G177" s="2">
         <v>43647</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:7">
       <c r="A178" s="1">
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C178" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D178" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E178" s="2">
         <v>43655</v>
       </c>
-      <c r="F178" s="2">
+      <c r="G178" s="2">
         <v>43661</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:7">
       <c r="A179" s="1">
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D179" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E179" s="2">
         <v>43655</v>
       </c>
-      <c r="F179" s="2">
+      <c r="G179" s="2">
         <v>43661</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:7">
       <c r="A180" s="1">
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D180" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E180" s="2">
         <v>43678</v>
       </c>
-      <c r="F180" s="2">
+      <c r="G180" s="2">
         <v>43686</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:7">
       <c r="A181" s="1">
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C181" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D181" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E181" s="2">
         <v>43678</v>
       </c>
-      <c r="F181" s="2">
+      <c r="G181" s="2">
         <v>43686</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:7">
       <c r="A182" s="1">
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C182" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D182" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E182" s="2">
         <v>43678</v>
       </c>
-      <c r="F182" s="2">
+      <c r="G182" s="2">
         <v>43686</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:7">
       <c r="A183" s="1">
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D183" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E183" s="2">
         <v>43678</v>
       </c>
-      <c r="F183" s="2">
+      <c r="G183" s="2">
         <v>43686</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:7">
       <c r="A184" s="1">
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D184" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E184" s="2">
         <v>41528</v>
@@ -5156,18 +5162,18 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:7">
       <c r="A185" s="1">
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C185" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D185" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E185" s="2">
         <v>41528</v>
@@ -5176,18 +5182,18 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:7">
       <c r="A186" s="1">
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C186" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D186" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E186" s="2">
         <v>41528</v>
@@ -5196,18 +5202,18 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:7">
       <c r="A187" s="1">
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C187" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D187" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E187" s="2">
         <v>41528</v>
@@ -5216,58 +5222,58 @@
         <v>41537</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:7">
       <c r="A188" s="1">
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C188" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D188" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E188" s="2">
         <v>43335</v>
       </c>
-      <c r="F188" s="2">
+      <c r="G188" s="2">
         <v>43340</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:7">
       <c r="A189" s="1">
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D189" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E189" s="2">
         <v>43335</v>
       </c>
-      <c r="F189" s="2">
+      <c r="G189" s="2">
         <v>43340</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:7">
       <c r="A190" s="1">
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C190" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D190" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E190" s="2">
         <v>41263</v>
@@ -5276,18 +5282,18 @@
         <v>41274</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:7">
       <c r="A191" s="1">
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C191" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D191" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E191" s="2">
         <v>41263</v>

</xml_diff>